<commit_message>
Update: verbeterde Streamlit versie
</commit_message>
<xml_diff>
--- a/data/quizvragen.xlsx
+++ b/data/quizvragen.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\o.jansen\Desktop\Learnings\Doc_quiz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56A8D8-9718-4821-A34C-2DFF37472D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C667482E-5881-4B2F-A200-61EB4B7E747C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DC" sheetId="1" r:id="rId1"/>
-    <sheet name="AC" sheetId="2" r:id="rId2"/>
+    <sheet name="Wiskunde 3" sheetId="3" r:id="rId2"/>
+    <sheet name="AC" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="123">
   <si>
     <t>id</t>
   </si>
@@ -132,13 +133,271 @@
   </si>
   <si>
     <t>P = U \cdot I</t>
+  </si>
+  <si>
+    <t>Goniometrie</t>
+  </si>
+  <si>
+    <t>Wat is de formule voor sin(α) in een rechthoekige driehoek?</t>
+  </si>
+  <si>
+    <t>["overstaande / schuine", "aanliggende / schuine", "overstaande / aanliggende"]</t>
+  </si>
+  <si>
+    <t>sin(α) = overstaande / schuine</t>
+  </si>
+  <si>
+    <t>sin(α)=o/h</t>
+  </si>
+  <si>
+    <t>["sinus","basisformule"]</t>
+  </si>
+  <si>
+    <t>Wat is de formule voor cos(α)?</t>
+  </si>
+  <si>
+    <t>["overstaande / schuine", "aanliggende / schuine", "aanliggende / overstaande"]</t>
+  </si>
+  <si>
+    <t>cos(α) = aanliggende / schuine</t>
+  </si>
+  <si>
+    <t>cos(α)=a/h</t>
+  </si>
+  <si>
+    <t>["cosinus","basisformule"]</t>
+  </si>
+  <si>
+    <t>Wat is de formule voor tan(α)?</t>
+  </si>
+  <si>
+    <t>["aanliggende / overstaande", "overstaande / aanliggende", "schuine / overstaande"]</t>
+  </si>
+  <si>
+    <t>tan(α) = overstaande / aanliggende</t>
+  </si>
+  <si>
+    <t>tan(α)=o/a</t>
+  </si>
+  <si>
+    <t>["tangens","basisformule"]</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>De formule tan(α)=sin(α)/cos(α) is juist.</t>
+  </si>
+  <si>
+    <t>Fundamentele identiteit.</t>
+  </si>
+  <si>
+    <t>["identiteit","tangens"]</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>sin²(α)+cos²(α)=1 is een goniometrische identiteit.</t>
+  </si>
+  <si>
+    <t>Altijd waar, ongeacht α.</t>
+  </si>
+  <si>
+    <t>["identiteit","pytagoras"]</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>Bereken tan(45°)</t>
+  </si>
+  <si>
+    <t>tan(45°)=1</t>
+  </si>
+  <si>
+    <t>["tangens","hoek"]</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>Bereken sin(90°)</t>
+  </si>
+  <si>
+    <t>sin(90°)=1</t>
+  </si>
+  <si>
+    <t>["sinus","hoek"]</t>
+  </si>
+  <si>
+    <t>q8</t>
+  </si>
+  <si>
+    <t>Bereken cos(60°)</t>
+  </si>
+  <si>
+    <t>cos(60°)=0.5</t>
+  </si>
+  <si>
+    <t>["cosinus","hoek"]</t>
+  </si>
+  <si>
+    <t>q9</t>
+  </si>
+  <si>
+    <t>Wat is sin(30°)?</t>
+  </si>
+  <si>
+    <t>["0", "0.5", "0.866", "1"]</t>
+  </si>
+  <si>
+    <t>sin(30°)=0.5</t>
+  </si>
+  <si>
+    <t>q10</t>
+  </si>
+  <si>
+    <t>Wat is cos(30°)?</t>
+  </si>
+  <si>
+    <t>["0.866", "0.5", "0", "1"]</t>
+  </si>
+  <si>
+    <t>cos(30°)=√3/2≈0.866</t>
+  </si>
+  <si>
+    <t>q11</t>
+  </si>
+  <si>
+    <t>Wat is tan(60°)?</t>
+  </si>
+  <si>
+    <t>["1", "0.5", "1.73", "0.866"]</t>
+  </si>
+  <si>
+    <t>tan(60°)=√3≈1.73</t>
+  </si>
+  <si>
+    <t>q12</t>
+  </si>
+  <si>
+    <t>cos(90°)=0.</t>
+  </si>
+  <si>
+    <t>Juist — cos(90°)=0</t>
+  </si>
+  <si>
+    <t>q13</t>
+  </si>
+  <si>
+    <t>Bereken sin(0°)</t>
+  </si>
+  <si>
+    <t>sin(0°)=0</t>
+  </si>
+  <si>
+    <t>q14</t>
+  </si>
+  <si>
+    <t>Wat is de formule om een zijde te berekenen bij een rechte driehoek met bekende hoek en schuine zijde?</t>
+  </si>
+  <si>
+    <t>["sinusregel", "cosinusregel", "tangensregel"]</t>
+  </si>
+  <si>
+    <t>overstaande = schuine * sin(α)</t>
+  </si>
+  <si>
+    <t>["sinus","berekening"]</t>
+  </si>
+  <si>
+    <t>q15</t>
+  </si>
+  <si>
+    <t>Wat is de cosinusregel?</t>
+  </si>
+  <si>
+    <t>["a²=b²+c²-2bc·cos(A)", "a²=b²+c²+2bc·cos(A)", "a²=b²-c²+2bc·cos(A)"]</t>
+  </si>
+  <si>
+    <t>cosinusregel</t>
+  </si>
+  <si>
+    <t>a²=b²+c²−2bc·cos(A)</t>
+  </si>
+  <si>
+    <t>["cosinusregel"]</t>
+  </si>
+  <si>
+    <t>q16</t>
+  </si>
+  <si>
+    <t>Wat is de sinusregel?</t>
+  </si>
+  <si>
+    <t>["a/sin(A)=b/sin(B)=c/sin(C)", "a·sin(A)=b·sin(B)", "a/b=sin(A)/sin(B)"]</t>
+  </si>
+  <si>
+    <t>sinusregel</t>
+  </si>
+  <si>
+    <t>a/sin(A)=b/sin(B)=c/sin(C)</t>
+  </si>
+  <si>
+    <t>["sinusregel"]</t>
+  </si>
+  <si>
+    <t>q17</t>
+  </si>
+  <si>
+    <t>Bereken de hoogte h in een driehoek met zijde c=10 en hoek A=30°: h=c·sin(A)</t>
+  </si>
+  <si>
+    <t>h=10·sin(30°)=5</t>
+  </si>
+  <si>
+    <t>["sinus","toepassing"]</t>
+  </si>
+  <si>
+    <t>q18</t>
+  </si>
+  <si>
+    <t>In de eenheidscirkel is de x-coördinaat gelijk aan de cosinuswaarde.</t>
+  </si>
+  <si>
+    <t>cos(x) = x-as</t>
+  </si>
+  <si>
+    <t>["eenheidscirkel","cosinus"]</t>
+  </si>
+  <si>
+    <t>q19</t>
+  </si>
+  <si>
+    <t>In de eenheidscirkel is de y-coördinaat gelijk aan de tangens.</t>
+  </si>
+  <si>
+    <t>Nee, dat is de sinus.</t>
+  </si>
+  <si>
+    <t>["eenheidscirkel","tangens"]</t>
+  </si>
+  <si>
+    <t>q20</t>
+  </si>
+  <si>
+    <t>Bereken cos(45°) afgerond op 2 decimalen.</t>
+  </si>
+  <si>
+    <t>cos(45°)=√2/2≈0.71</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +409,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,9 +454,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -496,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,6 +924,603 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05726C55-F5E0-4CC4-AAC4-7E0AD785995B}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>94</v>
+      </c>
+      <c r="J15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J16" t="s">
+        <v>101</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" t="s">
+        <v>111</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>114</v>
+      </c>
+      <c r="J19" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>118</v>
+      </c>
+      <c r="J20" t="s">
+        <v>119</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" t="s">
+        <v>122</v>
+      </c>
+      <c r="J21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Quizvragen aangepast via Admin
</commit_message>
<xml_diff>
--- a/data/quizvragen.xlsx
+++ b/data/quizvragen.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +491,11 @@
           <t>difficulty</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>image_url</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -544,6 +549,7 @@
       <c r="K2" t="n">
         <v>2</v>
       </c>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -597,6 +603,7 @@
       <c r="K3" t="n">
         <v>1</v>
       </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -650,6 +657,7 @@
       <c r="K4" t="n">
         <v>3</v>
       </c>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -677,6 +685,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -689,7 +698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -753,6 +762,11 @@
           <t>difficulty</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>image_url</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -772,12 +786,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Wat is de formule voor sin(α) in een rechthoekige driehoek?</t>
+          <t>Wat is de juiste formule voor de stroom I?</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>["overstaande / schuine", "aanliggende / schuine", "overstaande / aanliggende"]</t>
+          <t>['I = U/R', ' U = I*R', ' R = U/I']</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -802,6 +816,11 @@
       <c r="K2" t="n">
         <v>1</v>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>https://raw.githubusercontent.com/onomatorHanze/didactic-octo-spork/main/data/images/Wiskunde_3_q0_1763116823.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -851,6 +870,7 @@
       <c r="K3" t="n">
         <v>1</v>
       </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -900,6 +920,7 @@
       <c r="K4" t="n">
         <v>1</v>
       </c>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -941,6 +962,7 @@
       <c r="K5" t="n">
         <v>1</v>
       </c>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -982,6 +1004,7 @@
       <c r="K6" t="n">
         <v>2</v>
       </c>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1021,6 +1044,7 @@
       <c r="K7" t="n">
         <v>1</v>
       </c>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1060,6 +1084,7 @@
       <c r="K8" t="n">
         <v>1</v>
       </c>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1099,6 +1124,7 @@
       <c r="K9" t="n">
         <v>1</v>
       </c>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1144,6 +1170,7 @@
       <c r="K10" t="n">
         <v>1</v>
       </c>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1189,6 +1216,7 @@
       <c r="K11" t="n">
         <v>1</v>
       </c>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1234,6 +1262,7 @@
       <c r="K12" t="n">
         <v>1</v>
       </c>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1275,6 +1304,7 @@
       <c r="K13" t="n">
         <v>1</v>
       </c>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1314,6 +1344,7 @@
       <c r="K14" t="n">
         <v>1</v>
       </c>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1359,6 +1390,7 @@
       <c r="K15" t="n">
         <v>2</v>
       </c>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1408,6 +1440,7 @@
       <c r="K16" t="n">
         <v>3</v>
       </c>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1457,6 +1490,7 @@
       <c r="K17" t="n">
         <v>3</v>
       </c>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1496,6 +1530,7 @@
       <c r="K18" t="n">
         <v>2</v>
       </c>
+      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1537,6 +1572,7 @@
       <c r="K19" t="n">
         <v>2</v>
       </c>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1578,6 +1614,7 @@
       <c r="K20" t="n">
         <v>2</v>
       </c>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1617,6 +1654,7 @@
       <c r="K21" t="n">
         <v>1</v>
       </c>
+      <c r="L21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1629,7 +1667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1693,6 +1731,11 @@
           <t>difficulty</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>image_url</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1738,6 +1781,7 @@
       <c r="K2" t="n">
         <v>1</v>
       </c>
+      <c r="L2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update quizvragen via Admin
</commit_message>
<xml_diff>
--- a/data/quizvragen.xlsx
+++ b/data/quizvragen.xlsx
@@ -520,7 +520,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['I = U/R', '    U = I*R', '    R = U/I']</t>
+          <t>['I = U/R', '     U = I*R', '     R = U/I']</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -549,7 +549,11 @@
       <c r="K2" t="n">
         <v>2</v>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>https://raw.githubusercontent.com/onomatorHanze/didactic-octo-spork/main/data/images/DC_q0_1763125715.png</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>

<commit_message>
DocQuiz Admin – update vragenbestand
</commit_message>
<xml_diff>
--- a/data/quizvragen.xlsx
+++ b/data/quizvragen.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -674,38 +674,6 @@
       <c r="L5" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/onomatorHanze/didactic-octo-spork/main/data/images/DC_edit_4_1763134275.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>mc</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Werkt het toevoegen nu?</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>['test', 'test1', 'test2']</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>https://raw.githubusercontent.com/onomatorHanze/didactic-octo-spork/main/data/images/DC_new_1763462160.JPEG</t>
         </is>
       </c>
     </row>

</xml_diff>